<commit_message>
Add screenshot, update excel and README files
</commit_message>
<xml_diff>
--- a/export/sydney-restaurants-excel.xlsx
+++ b/export/sydney-restaurants-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Binyoh\Documents\Binyoh Coding Projects\Web Scraping Projects\Sydney-Restaurants-Scraper\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999D7D4-C2FB-4D44-AFDE-7B5973D8F1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B263F1-41A5-49A0-AC2B-52F30467E12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -14833,6 +14833,23 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -14858,23 +14875,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -19677,13 +19677,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:colOff>207530</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:colOff>359930</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -19700,8 +19700,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3954780" y="259080"/>
-          <a:ext cx="1371600" cy="731520"/>
+          <a:off x="3865130" y="255494"/>
+          <a:ext cx="1371600" cy="717177"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -19788,13 +19788,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:colOff>497090</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:colOff>39890</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -19811,8 +19811,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5463540" y="259080"/>
-          <a:ext cx="1371600" cy="731520"/>
+          <a:off x="5373890" y="255494"/>
+          <a:ext cx="1371600" cy="717177"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -19947,8 +19947,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>109729</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="8" name="Suburb">
@@ -19971,7 +19971,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -20025,8 +20025,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>109729</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="Style">
@@ -20049,7 +20049,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -20093,13 +20093,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:colOff>205287</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>412376</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>109728</xdr:rowOff>
     </xdr:to>
@@ -20137,8 +20137,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7117080" y="0"/>
-              <a:ext cx="3337560" cy="1389888"/>
+              <a:off x="6910887" y="0"/>
+              <a:ext cx="2645489" cy="1364787"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -32486,31 +32486,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A3F9EE9-8A7D-4D1B-A127-4F16CF3D8FF6}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A45:C62" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-  </pivotFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62707BE1-9791-44ED-9DD2-AD486B0EC9EA}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62707BE1-9791-44ED-9DD2-AD486B0EC9EA}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A22:B40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -33610,8 +33586,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{76C3FC11-9E69-44EF-93DC-36F28094D2A0}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{76C3FC11-9E69-44EF-93DC-36F28094D2A0}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -33972,6 +33948,30 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A3F9EE9-8A7D-4D1B-A127-4F16CF3D8FF6}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A45:C62" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Suburb" xr10:uid="{B2BB3439-F67D-46B6-B395-50E9DF02D49B}" sourceName="Suburb">
   <pivotTables>
@@ -34237,7 +34237,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84478B8C-423E-453D-87BB-E08E3FB417BE}" name="sydney_restaurants" displayName="sydney_restaurants" ref="A1:G1248" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84478B8C-423E-453D-87BB-E08E3FB417BE}" name="sydney_restaurants" displayName="sydney_restaurants" ref="A1:G1248" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:G1248" xr:uid="{84478B8C-423E-453D-87BB-E08E3FB417BE}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D86CD8FC-B05B-401B-B41F-48000CE7873F}" name="Name"/>
@@ -34246,7 +34246,7 @@
     <tableColumn id="4" xr3:uid="{DAA82416-448D-4618-AD67-6B030FBEBDAA}" name="Style"/>
     <tableColumn id="5" xr3:uid="{B36590F3-FBCE-4791-94FD-B662D09A462F}" name="Phone Number"/>
     <tableColumn id="6" xr3:uid="{9F183E77-7F63-47CF-A568-73CED3DFD18A}" name="Website"/>
-    <tableColumn id="7" xr3:uid="{5BCA4B5C-5504-4428-BFCE-B3CA0F84D265}" name="Date Published" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{5BCA4B5C-5504-4428-BFCE-B3CA0F84D265}" name="Date Published" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -34556,8 +34556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B6F7E1-8601-4243-86CE-C33011460A7A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>